<commit_message>
Ajout d'un nom pour les Corpus, Dossier : tjs sur Corpus
</commit_message>
<xml_diff>
--- a/dossiers/Domaines.xlsx
+++ b/dossiers/Domaines.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="27360" windowHeight="6720"/>
+    <workbookView xWindow="600" yWindow="120" windowWidth="27360" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Domaines" sheetId="1" r:id="rId1"/>
+    <sheet name="Niveau 0" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="By7g_WIa" localSheetId="0">Feuil1!$A$1:$C$394</definedName>
+    <definedName name="By7g_WIa" localSheetId="0">Domaines!$A$1:$C$394</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="788">
   <si>
     <t>docid</t>
   </si>
@@ -2747,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C394"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="B398" sqref="B398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7096,24 +7095,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>357</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>162</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>167</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>171</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>193</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>296</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>324</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>347</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>